<commit_message>
close #124: Add function to validate sequential codes in spreadsheet
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/descricao.xlsx
+++ b/input_data/data_ground_truth_01/descricao.xlsx
@@ -407,13 +407,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.43"/>
@@ -478,7 +477,7 @@
     </row>
     <row r="2" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>1</v>
@@ -524,8 +523,8 @@
       <c r="Y2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>5000</v>
+      <c r="A3" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>2</v>
@@ -571,8 +570,8 @@
       <c r="Y3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>5001</v>
+      <c r="A4" s="6" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>3</v>
@@ -618,8 +617,8 @@
       <c r="Y4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>5002</v>
+      <c r="A5" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>3</v>
@@ -665,8 +664,8 @@
       <c r="Y5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>5003</v>
+      <c r="A6" s="6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
@@ -712,8 +711,8 @@
       <c r="Y6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>5004</v>
+      <c r="A7" s="6" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>4</v>
@@ -759,8 +758,8 @@
       <c r="Y7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>5005</v>
+      <c r="A8" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>4</v>
@@ -806,8 +805,8 @@
       <c r="Y8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>5006</v>
+      <c r="A9" s="6" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>5</v>
@@ -853,8 +852,8 @@
       <c r="Y9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>5007</v>
+      <c r="A10" s="6" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
close #125: Correct mandatory value columns assumptions in valores.xlsx
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/descricao.xlsx
+++ b/input_data/data_ground_truth_01/descricao.xlsx
@@ -404,13 +404,13 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>

</xml_diff>

<commit_message>
close #122: Add  column as optional
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/descricao.xlsx
+++ b/input_data/data_ground_truth_01/descricao.xlsx
@@ -163,7 +163,7 @@
     <t xml:space="preserve">Produção e comercialização de alimentos</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensibilidade do sistema socioecológico quanto à disponibilidade de alimento e as possíveis limitações na sua comercialização no presente e no futuro considerando uma situação de seca.</t>
+    <t xml:space="preserve">Capacidade do sistema socioecológico de se ajustar a possíveis ameaças climáticas de seca teste 4.</t>
   </si>
   <si>
     <t xml:space="preserve">Sensibilidade do sistema quanto à disponibilidade de alimento e as possíveis limitações na sua comercialização no presente e no futuro considerando uma situação de seca. Essa informação é resultante da composição dos indicadores: baixa produção de alimentos básicos e não diversificação da produção local.&lt;br&gt;&lt;br&gt;Fonte:&lt;br&gt;Sistema de Informações e Análises sobre Impactos das Mudanças Climáticas – AdaptaBrasil MCTI.</t>
@@ -404,13 +404,13 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>

</xml_diff>